<commit_message>
changed sign up and login database to sql again
</commit_message>
<xml_diff>
--- a/database/reports/erfangh/Costs.xlsx
+++ b/database/reports/erfangh/Costs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,128 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1222</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2000/12/23</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>lmao</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024/06/01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>121212</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2000/12/22</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sdaffafaasdf</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024/06/01</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>12121221</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2000/12/22</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>erfan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024/05/27</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>23111</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2000/12/22</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>asdffdassdf</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024/05/30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>